<commit_message>
Latest support feeder 3.0
</commit_message>
<xml_diff>
--- a/upload/sample/sample_mhs_baru.xlsx
+++ b/upload/sample/sample_mhs_baru.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\feeder\upload\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\feeder-production\upload\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20391" windowHeight="8368"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2853,12 +2853,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="AU1" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ket : Jumlah Biaya Masuk Mahasiswa, isi tanpa koma atau titik.
+contoh : 5000000</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Info :  ini boleh kosong</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>NIM</t>
   </si>
@@ -2995,9 +3020,6 @@
     <t>Penghasilan Wali</t>
   </si>
   <si>
-    <t>ucok dadang</t>
-  </si>
-  <si>
     <t>Subang</t>
   </si>
   <si>
@@ -3029,6 +3051,12 @@
   </si>
   <si>
     <t>Jenis Pembiayaan</t>
+  </si>
+  <si>
+    <t>Jumlah Biaya Masuk</t>
+  </si>
+  <si>
+    <t>wildan tea</t>
   </si>
 </sst>
 </file>
@@ -3526,55 +3554,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT5"/>
+  <dimension ref="A1:AU5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AS5" sqref="AS5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.875" customWidth="1"/>
-    <col min="2" max="2" width="25.75" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="6" width="15.625" customWidth="1"/>
+    <col min="5" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="9" max="9" width="19.875" customWidth="1"/>
-    <col min="11" max="11" width="17.625" customWidth="1"/>
-    <col min="12" max="12" width="20.25" customWidth="1"/>
-    <col min="13" max="13" width="16.125" customWidth="1"/>
-    <col min="14" max="14" width="15.75" customWidth="1"/>
-    <col min="15" max="15" width="11.375" customWidth="1"/>
-    <col min="18" max="18" width="11.875" customWidth="1"/>
-    <col min="19" max="20" width="12.75" customWidth="1"/>
-    <col min="21" max="21" width="14.625" customWidth="1"/>
-    <col min="22" max="22" width="12.375" customWidth="1"/>
-    <col min="23" max="23" width="17.625" customWidth="1"/>
-    <col min="24" max="24" width="13.75" customWidth="1"/>
-    <col min="25" max="25" width="12.875" customWidth="1"/>
-    <col min="26" max="26" width="11.875" customWidth="1"/>
-    <col min="27" max="27" width="13.75" customWidth="1"/>
-    <col min="28" max="29" width="11.75" customWidth="1"/>
-    <col min="30" max="30" width="11.625" customWidth="1"/>
-    <col min="31" max="31" width="13.125" customWidth="1"/>
-    <col min="32" max="32" width="15.625" customWidth="1"/>
-    <col min="33" max="33" width="14.875" customWidth="1"/>
-    <col min="34" max="35" width="16.875" customWidth="1"/>
-    <col min="36" max="36" width="19.25" customWidth="1"/>
-    <col min="37" max="37" width="17.25" customWidth="1"/>
-    <col min="38" max="38" width="16.25" customWidth="1"/>
-    <col min="39" max="39" width="17.375" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="19" max="20" width="12.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1"/>
+    <col min="23" max="23" width="17.5703125" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
+    <col min="27" max="27" width="13.7109375" customWidth="1"/>
+    <col min="28" max="29" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" customWidth="1"/>
+    <col min="32" max="32" width="15.5703125" customWidth="1"/>
+    <col min="33" max="33" width="14.85546875" customWidth="1"/>
+    <col min="34" max="35" width="16.85546875" customWidth="1"/>
+    <col min="36" max="36" width="19.28515625" customWidth="1"/>
+    <col min="37" max="37" width="17.28515625" customWidth="1"/>
+    <col min="38" max="38" width="16.28515625" customWidth="1"/>
+    <col min="39" max="39" width="17.42578125" customWidth="1"/>
     <col min="40" max="40" width="18" customWidth="1"/>
-    <col min="41" max="41" width="20.125" customWidth="1"/>
-    <col min="42" max="42" width="17.75" customWidth="1"/>
-    <col min="43" max="43" width="17.625" customWidth="1"/>
-    <col min="44" max="44" width="18.875" customWidth="1"/>
-    <col min="45" max="45" width="22.25" customWidth="1"/>
+    <col min="41" max="41" width="20.140625" customWidth="1"/>
+    <col min="42" max="42" width="17.7109375" customWidth="1"/>
+    <col min="43" max="43" width="17.5703125" customWidth="1"/>
+    <col min="44" max="44" width="18.85546875" customWidth="1"/>
+    <col min="45" max="45" width="22.28515625" customWidth="1"/>
     <col min="46" max="46" width="18" customWidth="1"/>
+    <col min="47" max="47" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3711,24 +3740,27 @@
         <v>44</v>
       </c>
       <c r="AT1" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU1" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1209705555</v>
+        <v>12097055567</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D2" s="4">
         <v>33076</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="3">
         <v>3343423423</v>
@@ -3746,19 +3778,19 @@
         <v>123456</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L2" s="8">
         <v>1</v>
       </c>
       <c r="M2" s="9">
-        <v>42065</v>
+        <v>43526</v>
       </c>
       <c r="N2" s="8">
-        <v>20151</v>
+        <v>20191</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P2" s="10">
         <v>1</v>
@@ -3767,13 +3799,13 @@
         <v>5</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="U2" s="3">
         <v>41284</v>
@@ -3786,10 +3818,10 @@
       </c>
       <c r="X2" s="3"/>
       <c r="Y2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z2" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="AA2" s="3">
         <v>0</v>
@@ -3799,7 +3831,7 @@
         <v>234234</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE2" s="4">
         <v>14358</v>
@@ -3817,7 +3849,7 @@
         <v>23423423</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AK2" s="4">
         <v>21935</v>
@@ -3836,11 +3868,14 @@
       <c r="AQ2" s="3"/>
       <c r="AR2" s="16"/>
       <c r="AS2" s="3"/>
-      <c r="AT2">
+      <c r="AT2" s="3">
         <v>1</v>
       </c>
+      <c r="AU2" s="3">
+        <v>5000000</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="T5" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest update support latest feeder
</commit_message>
<xml_diff>
--- a/upload/sample/sample_mhs_baru.xlsx
+++ b/upload/sample/sample_mhs_baru.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\feeder-production\upload\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unyiltea\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2874,7 +2874,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Info :  ini boleh kosong</t>
+Info :  Wajib Diisi</t>
         </r>
       </text>
     </comment>
@@ -3556,8 +3556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AU7" sqref="AU7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,7 +3742,7 @@
       <c r="AT1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="AU1" s="19" t="s">
+      <c r="AU1" s="1" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>